<commit_message>
Updated pom use v0.8.2 of the api, ExcelImport shows creation of components and integrations
</commit_message>
<xml_diff>
--- a/excel-import/src/main/resources/data.xlsx
+++ b/excel-import/src/main/resources/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24520" yWindow="740" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -142,11 +142,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Fulgt hyperkobling" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperkobling" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperkobling" xfId="5" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,13 +479,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -552,7 +552,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -566,7 +565,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Excel Import creates fields WIP
</commit_message>
<xml_diff>
--- a/excel-import/src/main/resources/data.xlsx
+++ b/excel-import/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Application</t>
   </si>
@@ -62,16 +62,10 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>maintainer=erik@ardoq.com</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>email</t>
+    <t>maintainer</t>
+  </si>
+  <si>
+    <t>erik@ardoq.com</t>
   </si>
 </sst>
 </file>
@@ -128,22 +122,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -478,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -565,7 +561,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -612,10 +608,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -623,7 +619,7 @@
     <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,19 +629,13 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -653,6 +643,7 @@
     <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated ardoq-api version and data.xlsx in excel-import for fields
</commit_message>
<xml_diff>
--- a/excel-import/src/main/resources/data.xlsx
+++ b/excel-import/src/main/resources/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Application</t>
   </si>
@@ -62,10 +62,16 @@
     <t>Data</t>
   </si>
   <si>
-    <t>maintainer</t>
-  </si>
-  <si>
-    <t>erik@ardoq.com</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Field type</t>
+  </si>
+  <si>
+    <t>maintainer=erik@ardoq.com</t>
+  </si>
+  <si>
+    <t>Field name=value</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -619,23 +625,29 @@
     <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>